<commit_message>
added sliders for R_ion and other parameters
</commit_message>
<xml_diff>
--- a/paperdata/0.001sun.xlsx
+++ b/paperdata/0.001sun.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokey\Documents\UROP\paperdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokey\Documents\UROP\cir_simu\paperdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C6E03-F9C7-40C6-BA26-F924DD6F7F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FCAD70-CAC5-415C-8358-0F35F138FFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="990" windowWidth="28800" windowHeight="17910" xr2:uid="{E4322129-3D96-4C73-B3B4-BC2E8BC65296}"/>
+    <workbookView xWindow="1050" yWindow="3090" windowWidth="28815" windowHeight="17910" xr2:uid="{E4322129-3D96-4C73-B3B4-BC2E8BC65296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -451,7 +451,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F2" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -471,7 +471,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F3" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -491,7 +491,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F4" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -511,7 +511,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F5" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -531,7 +531,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F6" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -551,7 +551,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F7" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -571,7 +571,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F8" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -591,7 +591,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F9" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -611,7 +611,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F10" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -631,7 +631,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F11" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -651,7 +651,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F12" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -671,7 +671,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F13" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -691,7 +691,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F14" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -711,7 +711,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F15" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -731,7 +731,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F16" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -751,7 +751,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F17" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -771,7 +771,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F18" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -791,7 +791,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F19" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -811,7 +811,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F20" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -831,7 +831,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F21" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -851,7 +851,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F22" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -871,7 +871,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F23" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -891,7 +891,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F24" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -911,7 +911,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F25" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -931,7 +931,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F26" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -951,7 +951,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F27" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -971,7 +971,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F28" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -991,7 +991,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F29" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1011,7 +1011,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F30" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1031,7 +1031,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F31" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1051,7 +1051,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F32" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1071,7 +1071,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F33" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1091,7 +1091,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F34" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1111,7 +1111,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F35" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1131,7 +1131,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F36" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1151,7 +1151,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="F37" s="1">
-        <v>2.2000000000000001E-7</v>
+        <v>2.1999999999999999E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>